<commit_message>
upd 14.10 - 23.10
Методы оптимизации - лекция
Системный анализ - 3 лаба
</commit_message>
<xml_diff>
--- a/Системный анализ/Лаб 3/lab3_Структурная сложность(Системный анализ).xlsx
+++ b/Системный анализ/Лаб 3/lab3_Структурная сложность(Системный анализ).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80921CBB-5C0C-4D12-B2A3-511D49E9DFC4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ED2479-77D6-4B19-91D4-D9E706331B15}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1734,12 +1734,12 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -1764,13 +1764,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1778,13 +1778,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1809,10 +1809,10 @@
         <v>35</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1823,10 +1823,10 @@
         <v>43</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1837,10 +1837,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1851,38 +1851,38 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
+      <c r="B9" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>41</v>
+      <c r="B10" t="s">
+        <v>39</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1893,10 +1893,10 @@
         <v>33</v>
       </c>
       <c r="C11">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1910,7 +1910,7 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1921,7 +1921,7 @@
         <v>37</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -1935,7 +1935,7 @@
         <v>31</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -1946,13 +1946,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1960,13 +1960,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C16">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D16">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2001,28 +2001,28 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>23</v>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>19</v>
+      <c r="B20" t="s">
+        <v>23</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D20">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2054,7 +2054,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B22">
+  <sortState ref="A2:D22">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>